<commit_message>
Safetey measures for folder deletion
</commit_message>
<xml_diff>
--- a/NBi.Testing/Unit/Core/Excel/DataTableTest.xlsx
+++ b/NBi.Testing/Unit/Core/Excel/DataTableTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>*</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Tolerance</t>
-  </si>
-  <si>
-    <t>Global Tolerance</t>
   </si>
   <si>
     <t>RoundingStyle</t>
@@ -566,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,13 +583,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -600,25 +597,25 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
+      <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
@@ -632,160 +629,155 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F10" t="s">
-        <v>24</v>
+      <c r="F10" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>26</v>
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" t="s">
         <v>24</v>
       </c>
-      <c r="G11">
-        <v>1</v>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="F13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="9"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" s="4"/>
@@ -801,11 +793,6 @@
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" s="4"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>